<commit_message>
Add MoMA Linguistic Objects; homepages; images
</commit_message>
<xml_diff>
--- a/data/moma/source data/MoMAOKeeffeObjects.xlsx
+++ b/data/moma/source data/MoMAOKeeffeObjects.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="275">
   <si>
     <t>ObjectID</t>
   </si>
@@ -831,22 +831,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Pastel on paper mounted on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>board</t>
-    </r>
-  </si>
-  <si>
     <t>Photograph; platinum print</t>
   </si>
   <si>
@@ -881,7 +865,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,6 +899,14 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1003,11 +995,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1098,7 +1091,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1111,9 +1103,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1134,8 +1123,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Constituents" xfId="1"/>
   </cellStyles>
@@ -1439,8 +1432,8 @@
   <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W2" sqref="W2"/>
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1461,17 +1454,18 @@
     <col min="14" max="14" width="25.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="97" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="97" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="45.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="65.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="85.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="68.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="255.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="85.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="68.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="255.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="65.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="117.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="44.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="136.7109375" style="7" bestFit="1" customWidth="1"/>
@@ -1503,11 +1497,11 @@
       <c r="O1" s="27"/>
       <c r="P1" s="28"/>
       <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
+      <c r="R1" s="29"/>
       <c r="S1" s="25"/>
       <c r="T1" s="25"/>
       <c r="U1" s="25"/>
-      <c r="V1" s="29"/>
+      <c r="V1" s="25"/>
       <c r="W1" s="25"/>
       <c r="X1" s="29"/>
       <c r="Y1" s="29"/>
@@ -1569,22 +1563,22 @@
         <v>262</v>
       </c>
       <c r="R2" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="S2" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="S2" s="31" t="s">
-        <v>269</v>
-      </c>
       <c r="T2" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="U2" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="V2" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="V2" s="31" t="s">
+      <c r="W2" s="32" t="s">
         <v>274</v>
-      </c>
-      <c r="W2" s="32" t="s">
-        <v>275</v>
       </c>
       <c r="X2" s="35" t="s">
         <v>8</v>
@@ -1599,7 +1593,7 @@
         <v>272</v>
       </c>
       <c r="AB2" s="35" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="AC2" s="35" t="s">
         <v>13</v>
@@ -1612,25 +1606,25 @@
       </c>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
+      <c r="A3" s="36">
         <v>33250</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="39">
         <v>19.1936</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="42">
         <v>1934</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
@@ -1642,10 +1636,10 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="51">
+      <c r="M3" s="49">
         <v>13163</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O3" s="7" t="s">
@@ -1654,63 +1648,63 @@
       <c r="P3" s="9">
         <v>8901</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="Q3" s="36" t="s">
         <v>18</v>
       </c>
       <c r="R3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="37">
+      <c r="U3" s="36">
         <v>48.3</v>
       </c>
-      <c r="U3" s="37">
+      <c r="V3" s="36">
         <v>63.8</v>
       </c>
-      <c r="V3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AD3" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="AE3" s="7" t="s">
+      <c r="AE3" s="51" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
+      <c r="A4" s="36">
         <v>33281</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="39">
         <v>21.1936</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="42">
         <v>1934</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -1722,10 +1716,10 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="51">
+      <c r="M4" s="49">
         <v>13163</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O4" s="7" t="s">
@@ -1734,66 +1728,66 @@
       <c r="P4" s="9">
         <v>8901</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="36" t="s">
         <v>18</v>
       </c>
       <c r="R4" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="T4" s="37">
+      <c r="U4" s="36">
         <v>55.2</v>
       </c>
-      <c r="U4" s="37">
+      <c r="V4" s="36">
         <v>37.5</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="X4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Y4" s="11" t="s">
+      <c r="Y4" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="Z4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AD4" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="AE4" s="7" t="s">
+      <c r="AE4" s="51" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
+      <c r="A5" s="36">
         <v>78656</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="39">
         <v>65.1995</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="42">
         <v>1919</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -1805,10 +1799,10 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="51">
+      <c r="M5" s="49">
         <v>34736</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O5" s="7" t="s">
@@ -1817,63 +1811,63 @@
       <c r="P5" s="9">
         <v>8901</v>
       </c>
-      <c r="Q5" s="37" t="s">
+      <c r="Q5" s="36" t="s">
         <v>22</v>
       </c>
       <c r="R5" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="T5" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="T5" s="37">
+      <c r="U5" s="36">
         <v>69.5</v>
       </c>
-      <c r="U5" s="37">
+      <c r="V5" s="36">
         <v>59.1</v>
       </c>
-      <c r="V5" s="7" t="s">
-        <v>76</v>
+      <c r="Y5" s="37" t="s">
+        <v>77</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="37" t="s">
         <v>78</v>
       </c>
       <c r="AC5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" s="7" t="s">
+      <c r="AD5" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AE5" s="51" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
+      <c r="A6" s="36">
         <v>78677</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>71.197900000000004</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="42">
         <v>1927</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -1885,10 +1879,10 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="51">
+      <c r="M6" s="49">
         <v>28927</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O6" s="7" t="s">
@@ -1897,29 +1891,29 @@
       <c r="P6" s="9">
         <v>8901</v>
       </c>
-      <c r="Q6" s="37" t="s">
+      <c r="Q6" s="36" t="s">
         <v>22</v>
       </c>
       <c r="R6" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="37">
+      <c r="U6" s="36">
         <v>102.1</v>
       </c>
-      <c r="U6" s="37">
+      <c r="V6" s="36">
         <v>76</v>
       </c>
-      <c r="V6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y6" s="11" t="s">
-        <v>14</v>
+      <c r="Y6" s="37" t="s">
+        <v>53</v>
       </c>
       <c r="Z6" s="11" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="AA6" s="11" t="s">
         <v>14</v>
@@ -1927,33 +1921,33 @@
       <c r="AB6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AD6" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AE6" s="51" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
+      <c r="A7" s="36">
         <v>33828</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>91.195800000000006</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="42">
         <v>1917</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -1965,10 +1959,10 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="51">
+      <c r="M7" s="49">
         <v>21297</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O7" s="7" t="s">
@@ -1977,64 +1971,64 @@
       <c r="P7" s="9">
         <v>8901</v>
       </c>
-      <c r="Q7" s="43" t="s">
+      <c r="Q7" s="41" t="s">
         <v>264</v>
       </c>
       <c r="R7" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="T7" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="37">
+      <c r="U7" s="36">
         <v>22.5</v>
       </c>
-      <c r="U7" s="37">
+      <c r="V7" s="36">
         <v>30.2</v>
       </c>
-      <c r="V7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y7" s="11" t="s">
+      <c r="Y7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB7" s="37" t="s">
         <v>32</v>
-      </c>
-      <c r="Z7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="AC7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AD7" s="7" t="s">
+      <c r="AD7" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="AE7" s="7" t="s">
+      <c r="AE7" s="51" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+      <c r="A8" s="36">
         <v>34086</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="39">
         <v>113.1979</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="42">
         <v>1916</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -2046,10 +2040,10 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="51">
+      <c r="M8" s="49">
         <v>28982</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O8" s="7" t="s">
@@ -2058,66 +2052,66 @@
       <c r="P8" s="9">
         <v>8901</v>
       </c>
-      <c r="Q8" s="37" t="s">
+      <c r="Q8" s="36" t="s">
         <v>55</v>
       </c>
       <c r="R8" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="T8" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="T8" s="37">
+      <c r="U8" s="36">
         <v>30.3</v>
       </c>
-      <c r="U8" s="37">
+      <c r="V8" s="36">
         <v>22.5</v>
-      </c>
-      <c r="V8" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="X8" s="11" t="s">
         <v>58</v>
       </c>
       <c r="Y8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA8" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB8" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="Z8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD8" s="7" t="s">
+      <c r="AD8" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="AE8" s="7" t="s">
+      <c r="AE8" s="51" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="A9" s="36">
         <v>78978</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="39">
         <v>144.19450000000001</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -2129,10 +2123,10 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="51">
+      <c r="M9" s="49">
         <v>16553</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O9" s="7" t="s">
@@ -2141,54 +2135,54 @@
       <c r="P9" s="9">
         <v>8901</v>
       </c>
-      <c r="Q9" s="37" t="s">
+      <c r="Q9" s="36" t="s">
         <v>22</v>
       </c>
       <c r="R9" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="T9" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="T9" s="37">
+      <c r="U9" s="36">
         <v>101.6</v>
       </c>
-      <c r="U9" s="37">
+      <c r="V9" s="36">
         <v>76.2</v>
       </c>
-      <c r="V9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z9" s="11" t="s">
+      <c r="Y9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="AD9" s="7" t="s">
+      <c r="AD9" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="AE9" s="7" t="s">
+      <c r="AE9" s="51" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="36">
         <v>35245</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="39">
         <v>199.1995</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="42">
         <v>1919</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -2200,10 +2194,10 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="51">
+      <c r="M10" s="49">
         <v>34864</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O10" s="7" t="s">
@@ -2212,69 +2206,69 @@
       <c r="P10" s="9">
         <v>8901</v>
       </c>
-      <c r="Q10" s="37" t="s">
+      <c r="Q10" s="36" t="s">
         <v>18</v>
       </c>
       <c r="R10" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="S10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="T10" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="T10" s="37">
+      <c r="U10" s="36">
         <v>49.8476</v>
       </c>
-      <c r="U10" s="37">
+      <c r="V10" s="36">
         <v>32.385100000000001</v>
-      </c>
-      <c r="V10" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="X10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Y10" s="50" t="s">
+      <c r="Y10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB10" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="Z10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB10" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="AC10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD10" s="7" t="s">
+      <c r="AD10" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AE10" s="7" t="s">
+      <c r="AE10" s="51" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
+      <c r="A11" s="36">
         <v>35251</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="39">
         <v>200.1995</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="42">
         <v>1916</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -2286,10 +2280,10 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="51">
+      <c r="M11" s="49">
         <v>34864</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O11" s="7" t="s">
@@ -2298,63 +2292,63 @@
       <c r="P11" s="9">
         <v>8901</v>
       </c>
-      <c r="Q11" s="37" t="s">
+      <c r="Q11" s="36" t="s">
         <v>18</v>
       </c>
       <c r="R11" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="S11" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="T11" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="T11" s="37">
+      <c r="U11" s="36">
         <v>60.960099999999997</v>
       </c>
-      <c r="U11" s="37">
+      <c r="V11" s="36">
         <v>48.260100000000001</v>
       </c>
-      <c r="V11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y11" s="50" t="s">
+      <c r="Y11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA11" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB11" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="Z11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD11" s="7" t="s">
+      <c r="AD11" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="AE11" s="7" t="s">
+      <c r="AE11" s="51" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41">
+      <c r="A12" s="40">
         <v>91461</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="F12" s="39" t="s">
+      <c r="E12" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H12" s="13" t="s">
@@ -2373,7 +2367,7 @@
         <v>4360</v>
       </c>
       <c r="M12" s="12"/>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O12" s="7" t="s">
@@ -2382,68 +2376,68 @@
       <c r="P12" s="9">
         <v>8901</v>
       </c>
-      <c r="Q12" s="39" t="s">
+      <c r="Q12" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="R12" s="42" t="s">
+      <c r="R12" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="T12" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="T12" s="13"/>
       <c r="U12" s="13"/>
-      <c r="V12" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="V12" s="13"/>
       <c r="W12" s="13" t="s">
         <v>14</v>
       </c>
       <c r="X12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Y12" s="11" t="s">
-        <v>14</v>
+      <c r="Y12" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="Z12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA12" s="11" t="s">
-        <v>14</v>
+        <v>14</v>
+      </c>
+      <c r="AA12" s="37" t="s">
+        <v>104</v>
       </c>
       <c r="AB12" s="11" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="AC12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD12" s="7" t="s">
+      <c r="AD12" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AE12" s="52" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37">
+      <c r="A13" s="36">
         <v>35902</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="39">
         <v>277.19720000000001</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="42">
         <v>1959</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -2455,10 +2449,10 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="51">
+      <c r="M13" s="49">
         <v>26577</v>
       </c>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O13" s="7" t="s">
@@ -2467,63 +2461,63 @@
       <c r="P13" s="9">
         <v>8901</v>
       </c>
-      <c r="Q13" s="37" t="s">
+      <c r="Q13" s="36" t="s">
         <v>18</v>
       </c>
       <c r="R13" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="S13" s="7" t="s">
+      <c r="T13" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="T13" s="37">
+      <c r="U13" s="36">
         <v>63.2</v>
       </c>
-      <c r="U13" s="37">
+      <c r="V13" s="36">
         <v>47.3</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="X13" s="11" t="s">
         <v>47</v>
       </c>
       <c r="Y13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z13" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="Z13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD13" s="7" t="s">
+      <c r="AD13" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="AE13" s="7" t="s">
+      <c r="AE13" s="51" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37">
+      <c r="A14" s="36">
         <v>79714</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="39">
         <v>447.19940000000003</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="42">
         <v>1977</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -2535,10 +2529,10 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="51">
+      <c r="M14" s="49">
         <v>34618</v>
       </c>
-      <c r="N14" s="37" t="s">
+      <c r="N14" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O14" s="7" t="s">
@@ -2547,60 +2541,60 @@
       <c r="P14" s="9">
         <v>8901</v>
       </c>
-      <c r="Q14" s="37" t="s">
+      <c r="Q14" s="36" t="s">
         <v>22</v>
       </c>
       <c r="R14" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="S14" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="T14" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="T14" s="37">
+      <c r="U14" s="36">
         <v>121.9</v>
       </c>
-      <c r="U14" s="37">
+      <c r="V14" s="36">
         <v>91.4</v>
       </c>
-      <c r="V14" s="7" t="s">
-        <v>71</v>
+      <c r="Y14" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA14" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="AD14" s="7" t="s">
+      <c r="AD14" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="AE14" s="7" t="s">
+      <c r="AE14" s="51" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="36">
         <v>37328</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="42">
         <v>1941</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="36" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="7" t="s">
@@ -2612,10 +2606,10 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="51">
+      <c r="M15" s="49">
         <v>33171</v>
       </c>
-      <c r="N15" s="37" t="s">
+      <c r="N15" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O15" s="7" t="s">
@@ -2624,66 +2618,66 @@
       <c r="P15" s="9">
         <v>8901</v>
       </c>
-      <c r="Q15" s="43" t="s">
-        <v>265</v>
+      <c r="Q15" s="50" t="s">
+        <v>62</v>
       </c>
       <c r="R15" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="S15" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="T15" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="T15" s="37">
+      <c r="U15" s="36">
         <v>70.167599999999993</v>
       </c>
-      <c r="U15" s="37">
+      <c r="V15" s="36">
         <v>55.245100000000001</v>
-      </c>
-      <c r="V15" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="X15" s="11" t="s">
         <v>65</v>
       </c>
       <c r="Y15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z15" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA15" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB15" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Z15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB15" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD15" s="7" t="s">
+      <c r="AD15" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="AE15" s="7" t="s">
+      <c r="AE15" s="51" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41">
+      <c r="A16" s="40">
         <v>83915</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="E16" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="F16" s="39" t="s">
+      <c r="E16" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H16" s="13" t="s">
@@ -2702,7 +2696,7 @@
         <v>4360</v>
       </c>
       <c r="M16" s="12"/>
-      <c r="N16" s="37" t="s">
+      <c r="N16" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O16" s="7" t="s">
@@ -2711,25 +2705,25 @@
       <c r="P16" s="9">
         <v>8901</v>
       </c>
-      <c r="Q16" s="39" t="s">
+      <c r="Q16" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="R16" s="42" t="s">
+      <c r="R16" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="S16" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="S16" s="13" t="s">
+      <c r="T16" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="T16" s="39" t="s">
+      <c r="U16" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="U16" s="39" t="s">
+      <c r="V16" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="V16" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="W16" s="13" t="s">
+      <c r="W16" s="38" t="s">
         <v>95</v>
       </c>
       <c r="X16" s="11" t="s">
@@ -2741,40 +2735,40 @@
       <c r="Z16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AA16" s="11" t="s">
-        <v>14</v>
+      <c r="AA16" s="37" t="s">
+        <v>96</v>
       </c>
       <c r="AB16" s="11" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="AC16" s="11"/>
-      <c r="AD16" s="7" t="s">
+      <c r="AD16" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AE16" s="52" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41">
+      <c r="A17" s="40">
         <v>229012</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="F17" s="39" t="s">
+      <c r="E17" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H17" s="13" t="s">
@@ -2793,7 +2787,7 @@
         <v>4360</v>
       </c>
       <c r="M17" s="12"/>
-      <c r="N17" s="37" t="s">
+      <c r="N17" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O17" s="7" t="s">
@@ -2802,24 +2796,24 @@
       <c r="P17" s="9">
         <v>8901</v>
       </c>
-      <c r="Q17" s="39" t="s">
+      <c r="Q17" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="R17" s="42" t="s">
+      <c r="R17" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="S17" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="T17" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="39" t="s">
+      <c r="U17" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="U17" s="37">
+      <c r="V17" s="36">
         <v>13.8</v>
       </c>
-      <c r="V17" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="W17" s="13" t="s">
         <v>14</v>
       </c>
@@ -2841,30 +2835,30 @@
       <c r="AC17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD17" s="7" t="s">
+      <c r="AD17" s="51" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+      <c r="A18" s="40">
         <v>229013</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="F18" s="39" t="s">
+      <c r="E18" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F18" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="38" t="s">
         <v>111</v>
       </c>
       <c r="H18" s="13" t="s">
@@ -2883,7 +2877,7 @@
         <v>4360</v>
       </c>
       <c r="M18" s="12"/>
-      <c r="N18" s="37" t="s">
+      <c r="N18" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O18" s="7" t="s">
@@ -2892,24 +2886,24 @@
       <c r="P18" s="9">
         <v>8901</v>
       </c>
-      <c r="Q18" s="39" t="s">
+      <c r="Q18" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="R18" s="42" t="s">
+      <c r="R18" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="S18" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="S18" s="13" t="s">
+      <c r="T18" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="T18" s="39" t="s">
+      <c r="U18" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="U18" s="39" t="s">
+      <c r="V18" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="V18" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="W18" s="13" t="s">
         <v>14</v>
       </c>
@@ -2931,30 +2925,30 @@
       <c r="AC18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD18" s="7" t="s">
+      <c r="AD18" s="36" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41">
+      <c r="A19" s="40">
         <v>229014</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="38" t="s">
         <v>111</v>
       </c>
       <c r="H19" s="13" t="s">
@@ -2973,7 +2967,7 @@
         <v>4360</v>
       </c>
       <c r="M19" s="12"/>
-      <c r="N19" s="37" t="s">
+      <c r="N19" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O19" s="7" t="s">
@@ -2982,24 +2976,24 @@
       <c r="P19" s="9">
         <v>8901</v>
       </c>
-      <c r="Q19" s="39" t="s">
+      <c r="Q19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="R19" s="42" t="s">
+      <c r="R19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="S19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="S19" s="13" t="s">
+      <c r="T19" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="T19" s="39" t="s">
+      <c r="U19" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="U19" s="39" t="s">
+      <c r="V19" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="V19" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="W19" s="13" t="s">
         <v>14</v>
       </c>
@@ -3021,30 +3015,30 @@
       <c r="AC19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD19" s="7" t="s">
+      <c r="AD19" s="36" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41">
+      <c r="A20" s="40">
         <v>229015</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E20" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="F20" s="39" t="s">
+      <c r="E20" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="38" t="s">
         <v>111</v>
       </c>
       <c r="H20" s="13" t="s">
@@ -3063,7 +3057,7 @@
         <v>4360</v>
       </c>
       <c r="M20" s="12"/>
-      <c r="N20" s="37" t="s">
+      <c r="N20" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O20" s="7" t="s">
@@ -3072,24 +3066,24 @@
       <c r="P20" s="9">
         <v>8901</v>
       </c>
-      <c r="Q20" s="39" t="s">
+      <c r="Q20" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="R20" s="42" t="s">
+      <c r="R20" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="S20" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="S20" s="13" t="s">
+      <c r="T20" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="T20" s="39" t="s">
+      <c r="U20" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="U20" s="39" t="s">
+      <c r="V20" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="V20" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="W20" s="13" t="s">
         <v>14</v>
       </c>
@@ -3111,30 +3105,30 @@
       <c r="AC20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD20" s="7" t="s">
+      <c r="AD20" s="36" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41">
+      <c r="A21" s="40">
         <v>229016</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="F21" s="39" t="s">
+      <c r="E21" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F21" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H21" s="13" t="s">
@@ -3153,7 +3147,7 @@
         <v>4360</v>
       </c>
       <c r="M21" s="12"/>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O21" s="7" t="s">
@@ -3162,24 +3156,24 @@
       <c r="P21" s="9">
         <v>8901</v>
       </c>
-      <c r="Q21" s="39" t="s">
+      <c r="Q21" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="R21" s="42" t="s">
+      <c r="R21" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="S21" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="S21" s="13" t="s">
+      <c r="T21" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="T21" s="39" t="s">
+      <c r="U21" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="U21" s="39" t="s">
+      <c r="V21" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="V21" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="W21" s="13" t="s">
         <v>14</v>
       </c>
@@ -3201,30 +3195,30 @@
       <c r="AC21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD21" s="7" t="s">
+      <c r="AD21" s="36" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41">
+      <c r="A22" s="40">
         <v>229199</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="F22" s="39" t="s">
+      <c r="E22" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F22" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="38" t="s">
         <v>120</v>
       </c>
       <c r="H22" s="13" t="s">
@@ -3243,7 +3237,7 @@
         <v>181</v>
       </c>
       <c r="M22" s="12"/>
-      <c r="N22" s="37" t="s">
+      <c r="N22" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O22" s="7" t="s">
@@ -3252,24 +3246,24 @@
       <c r="P22" s="9">
         <v>8901</v>
       </c>
-      <c r="Q22" s="39" t="s">
+      <c r="Q22" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="R22" s="42" t="s">
+      <c r="R22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="S22" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="S22" s="13" t="s">
+      <c r="T22" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="T22" s="39" t="s">
+      <c r="U22" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="U22" s="39" t="s">
+      <c r="V22" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="V22" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="W22" s="13" t="s">
         <v>14</v>
       </c>
@@ -3291,30 +3285,30 @@
       <c r="AC22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD22" s="7" t="s">
+      <c r="AD22" s="36" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41">
+      <c r="A23" s="40">
         <v>33505</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="38" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="13" t="s">
@@ -3333,7 +3327,7 @@
         <v>16170</v>
       </c>
       <c r="M23" s="12"/>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="36" t="s">
         <v>215</v>
       </c>
       <c r="O23" s="7" t="s">
@@ -3342,46 +3336,46 @@
       <c r="P23" s="9">
         <v>8901</v>
       </c>
-      <c r="Q23" s="39" t="s">
+      <c r="Q23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="R23" s="42" t="s">
+      <c r="R23" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="S23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="T23" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="T23" s="39" t="s">
+      <c r="U23" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="U23" s="39" t="s">
+      <c r="V23" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="V23" s="11" t="s">
-        <v>129</v>
-      </c>
       <c r="W23" s="13" t="s">
         <v>14</v>
       </c>
       <c r="X23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Y23" s="50" t="s">
+      <c r="Y23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB23" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="Z23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB23" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="AC23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AD23" s="7" t="s">
+      <c r="AD23" s="36" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3394,8 +3388,39 @@
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="N1:P1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AE3" r:id="rId1"/>
+    <hyperlink ref="AD3" r:id="rId2"/>
+    <hyperlink ref="AD4" r:id="rId3"/>
+    <hyperlink ref="AE4" r:id="rId4"/>
+    <hyperlink ref="AD5" r:id="rId5"/>
+    <hyperlink ref="AE5" r:id="rId6"/>
+    <hyperlink ref="AD7" r:id="rId7"/>
+    <hyperlink ref="AD6" r:id="rId8"/>
+    <hyperlink ref="AE6" r:id="rId9"/>
+    <hyperlink ref="AE7" r:id="rId10"/>
+    <hyperlink ref="AD8" r:id="rId11"/>
+    <hyperlink ref="AE8" r:id="rId12"/>
+    <hyperlink ref="AD9" r:id="rId13"/>
+    <hyperlink ref="AE9" r:id="rId14"/>
+    <hyperlink ref="AD10" r:id="rId15"/>
+    <hyperlink ref="AE10" r:id="rId16"/>
+    <hyperlink ref="AD11" r:id="rId17"/>
+    <hyperlink ref="AE11" r:id="rId18"/>
+    <hyperlink ref="AD12" r:id="rId19"/>
+    <hyperlink ref="AE12" r:id="rId20"/>
+    <hyperlink ref="AD13" r:id="rId21"/>
+    <hyperlink ref="AE13" r:id="rId22"/>
+    <hyperlink ref="AD14" r:id="rId23"/>
+    <hyperlink ref="AE14" r:id="rId24"/>
+    <hyperlink ref="AD15" r:id="rId25"/>
+    <hyperlink ref="AE15" r:id="rId26"/>
+    <hyperlink ref="AD16" r:id="rId27"/>
+    <hyperlink ref="AE16" r:id="rId28"/>
+    <hyperlink ref="AD17" r:id="rId29" location="/detail/229012"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
@@ -3430,56 +3455,56 @@
     <col min="18" max="16384" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="49" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:17" s="47" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="46" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3566,7 +3591,7 @@
       <c r="B4" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="43" t="s">
         <v>236</v>
       </c>
       <c r="D4" s="13" t="s">

</xml_diff>